<commit_message>
add brand of segement
</commit_message>
<xml_diff>
--- a/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template_Rollout.xlsx
+++ b/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template_Rollout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="exclusion_rules" sheetId="1" state="visible" r:id="rId2"/>
@@ -83,9 +83,6 @@
     <t xml:space="preserve">Brand SOS</t>
   </si>
   <si>
-    <t xml:space="preserve">Sub Brand SOS</t>
-  </si>
-  <si>
     <t xml:space="preserve">PepsiCo Segment SOS</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t xml:space="preserve">BLACK COUNTRY SNACKS, AKSAM PALUSZKI, LAJKONIK PALUSZKI, ALKA ELEPHANT, RUMPLERS, TABITHA, CHEF'S LARDER, BOROMIR, COFRESH, JIFFY POP, CROCO, THE CURATORS, FRESHERS, FUDCO, GEFEN, GINNI'S, OH MY GURU!, HALDIRAMS, HALDIRAMS SNACKS, INDIE BAY SNACKS, INNATE, JACK-LNK'S, EAZY-PP-PPCRN, ZWEIFEL CRISPS, HUNKY DORYS CRISPS, LAJKONIK JUNIOR, LOVE CHIN CHIN, NISHAS SNACKS, NUTELLA, OSEM SAVOURY SNACK, OUR LITTLE REBELL!ON, EPIC, CRAWFORDS, FLIPZ, OATIS, RYMUT SNACKS, GINCO, SUNSHINE SNACKS, JAY'S, MIDLAND SNACKS, RED MILL SAVOURY SNACKS, SENSIBLE PORTIONS, VISCONTI SNACKS, WELL &amp; TRULY SNACKS, WILD WEST, WILDING'S, BLUE DRAGON, BEPPS, BLUE DIAMOND, COFRESH SNACKS, SCHAR, OLD EL PASO, PLANTERS, LINWOODS, CYPRESSA, KOHINOOR SNACKS, KOIKEYA, PALUSZKI, LORENZ CRISPS, MCCOLGAN, ITSU, NAIRNS, NATURES STORE SNACKS, NIM'S, BAMBA SNACKS, BISSLI SNACKS, SHARWOODS, MR PORKY SNACKS, TYGRYSKI, THE REAL PORK CRACKLING CO SNACKS, THE SNAFFLING PIG CO, WHITWORTHS, YUM &amp; YAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand SOS of Segment</t>
   </si>
   <si>
     <t xml:space="preserve">Price Scene</t>
@@ -316,18 +316,18 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.8825910931174"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.8825910931174"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.7368421052632"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -499,79 +499,79 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>13</v>
+      <c r="D13" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>18</v>
+      <c r="A14" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>11</v>
@@ -585,7 +585,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>11</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="20" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>11</v>
@@ -613,7 +613,7 @@
     </row>
     <row r="21" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>11</v>
@@ -643,14 +643,14 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.5627530364373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
@@ -692,11 +692,12 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="C5" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fix filtering for mainshelf
</commit_message>
<xml_diff>
--- a/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template_Rollout.xlsx
+++ b/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template_Rollout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="exclusion_rules" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="33">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ignore Store Policy</t>
   </si>
   <si>
     <t xml:space="preserve">All</t>
@@ -314,20 +317,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.2064777327935"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.7368421052632"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.2753036437247"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -344,285 +347,348 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>23</v>
+      <c r="E16" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -644,13 +710,13 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.5627530364373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
@@ -660,42 +726,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3"/>
     </row>

</xml_diff>

<commit_message>
add rule for empty
</commit_message>
<xml_diff>
--- a/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template_Rollout.xlsx
+++ b/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template_Rollout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="exclusion_rules" sheetId="1" state="visible" r:id="rId2"/>
@@ -458,17 +458,17 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C59" activeCellId="0" sqref="C59"/>
+      <selection pane="topLeft" activeCell="E57" activeCellId="0" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.3846153846154"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1295546558704"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.5587044534413"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1403,6 +1403,9 @@
       <c r="D55" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="E55" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
@@ -1416,6 +1419,9 @@
       </c>
       <c r="D56" s="0" t="s">
         <v>52</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1442,8 +1448,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5263157894737"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>

</xml_diff>

<commit_message>
change dsplay template and fix excl templ
</commit_message>
<xml_diff>
--- a/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template_Rollout.xlsx
+++ b/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template_Rollout.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="63">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -257,7 +257,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,6 +292,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF950E"/>
         <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FFFF"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -329,7 +335,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -374,6 +380,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -408,7 +418,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF99FFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -455,20 +465,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E57" activeCellId="0" sqref="E57"/>
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.0242914979757"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.5587044534413"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.5222672064777"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1170,7 +1180,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B42" s="8" t="s">
@@ -1187,7 +1197,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B43" s="8" t="s">
@@ -1204,7 +1214,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B44" s="0" t="s">
@@ -1221,7 +1231,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B45" s="9" t="s">
@@ -1238,7 +1248,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B46" s="0" t="s">
@@ -1254,37 +1264,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+    <row r="47" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D47" s="8" t="s">
+      <c r="B47" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E47" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E48" s="10" t="n">
+      <c r="E47" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E48" s="11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1292,16 +1302,16 @@
       <c r="A49" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E49" s="0" t="n">
+      <c r="B49" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E49" s="10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1309,31 +1319,31 @@
       <c r="A50" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E50" s="10" t="n">
+      <c r="B50" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>32</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E51" s="10" t="n">
         <v>1</v>
@@ -1343,33 +1353,33 @@
       <c r="A52" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E52" s="0" t="n">
+      <c r="B52" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E52" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E53" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E53" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1377,22 +1387,22 @@
       <c r="A54" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E54" s="0" t="n">
+      <c r="B54" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E54" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>6</v>
@@ -1409,7 +1419,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>6</v>
@@ -1421,6 +1431,23 @@
         <v>52</v>
       </c>
       <c r="E56" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1448,8 +1475,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.9554655870445"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
@@ -1458,10 +1485,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
move changes to prod
</commit_message>
<xml_diff>
--- a/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template_Rollout.xlsx
+++ b/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template_Rollout.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="64">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -56,6 +56,12 @@
     <t xml:space="preserve">additional display</t>
   </si>
   <si>
+    <t xml:space="preserve">product_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Irrelevant</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hero SKU Availability - SKU</t>
   </si>
   <si>
@@ -174,9 +180,6 @@
   </si>
   <si>
     <t xml:space="preserve">Secondary Brand Of Category SOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_type</t>
   </si>
   <si>
     <t xml:space="preserve">POS</t>
@@ -465,20 +468,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D7:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.3481781376518"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.5222672064777"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.0566801619433"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -533,35 +536,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
@@ -569,50 +572,50 @@
     </row>
     <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E6" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>18</v>
+      <c r="A8" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>1</v>
@@ -620,33 +623,33 @@
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>20</v>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>1</v>
@@ -654,16 +657,16 @@
     </row>
     <row r="11" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>1</v>
@@ -671,50 +674,50 @@
     </row>
     <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>19</v>
+    <row r="13" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>20</v>
+      <c r="A14" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>0</v>
@@ -722,16 +725,16 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>0</v>
@@ -739,50 +742,50 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="D16" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E17" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1</v>
@@ -790,16 +793,16 @@
     </row>
     <row r="19" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>1</v>
@@ -807,16 +810,16 @@
     </row>
     <row r="20" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>1</v>
@@ -824,33 +827,33 @@
     </row>
     <row r="21" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>31</v>
+    <row r="22" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>1</v>
@@ -858,13 +861,13 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>33</v>
@@ -875,13 +878,13 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>35</v>
@@ -895,10 +898,10 @@
         <v>36</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>37</v>
@@ -908,31 +911,31 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" s="9" t="n">
+      <c r="B26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>33</v>
@@ -943,15 +946,15 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>35</v>
       </c>
       <c r="E28" s="9" t="n">
@@ -960,15 +963,15 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>37</v>
       </c>
       <c r="E29" s="9" t="n">
@@ -976,31 +979,31 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E30" s="10" t="n">
+      <c r="A30" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>33</v>
@@ -1011,13 +1014,13 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>35</v>
@@ -1028,13 +1031,13 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>37</v>
@@ -1044,31 +1047,31 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" s="0" t="n">
+      <c r="A34" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>33</v>
@@ -1079,15 +1082,15 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D36" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>35</v>
       </c>
       <c r="E36" s="0" t="n">
@@ -1096,15 +1099,15 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D37" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="9" t="s">
         <v>37</v>
       </c>
       <c r="E37" s="0" t="n">
@@ -1113,30 +1116,30 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E38" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>33</v>
@@ -1147,13 +1150,13 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>35</v>
@@ -1164,13 +1167,13 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>37</v>
@@ -1180,31 +1183,31 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E42" s="0" t="n">
+      <c r="A42" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E42" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>33</v>
@@ -1215,16 +1218,16 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D44" s="0" t="s">
         <v>52</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>1</v>
@@ -1232,16 +1235,16 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>35</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>1</v>
@@ -1249,103 +1252,103 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E46" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E47" s="11" t="n">
+      <c r="E47" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E48" s="11" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+    <row r="49" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E49" s="10" t="n">
+      <c r="B49" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E49" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E50" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E50" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E51" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E51" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1354,10 +1357,10 @@
         <v>56</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D52" s="10" t="s">
         <v>35</v>
@@ -1368,18 +1371,18 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E53" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E53" s="10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1387,33 +1390,33 @@
       <c r="A54" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E54" s="10" t="n">
+      <c r="B54" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E54" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B55" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E55" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E55" s="10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1425,10 +1428,10 @@
         <v>6</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>1</v>
@@ -1442,12 +1445,29 @@
         <v>6</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E57" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E58" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1470,13 +1490,13 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="D7:D8 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.7044534412956"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.0242914979757"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
@@ -1486,42 +1506,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C5" s="3"/>
     </row>

</xml_diff>

<commit_message>
fix external targets template
</commit_message>
<xml_diff>
--- a/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template_Rollout.xlsx
+++ b/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template_Rollout.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="64">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -119,6 +119,9 @@
     <t xml:space="preserve">Linear Space Per Product</t>
   </si>
   <si>
+    <t xml:space="preserve">POS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Secondary Hero SKU Availability - SKU</t>
   </si>
   <si>
@@ -180,9 +183,6 @@
   </si>
   <si>
     <t xml:space="preserve">Secondary Brand Of Category SOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POS</t>
   </si>
   <si>
     <t xml:space="preserve">FTG Brand Of Category SOS</t>
@@ -468,20 +468,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D7:D8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.3481781376518"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.668016194332"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.0566801619433"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.5951417004049"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -842,502 +842,502 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="B26" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="6" t="s">
+      <c r="E26" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="B27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
+      <c r="E27" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="6" t="s">
+      <c r="E28" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
+      <c r="E31" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="E33" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="s">
+      <c r="E35" s="10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" s="9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E28" s="9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" s="9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E32" s="10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" s="10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" s="10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E35" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E36" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E37" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E40" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E41" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E44" s="10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E42" s="10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
+      <c r="B45" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45" s="10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E43" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E44" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E45" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E46" s="0" t="n">
+      <c r="B46" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E47" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E48" s="11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E49" s="11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E50" s="10" t="n">
+      <c r="B50" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E50" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>56</v>
+      <c r="A51" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>6</v>
@@ -1346,117 +1346,117 @@
         <v>11</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E52" s="10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E53" s="10" t="n">
+    <row r="52" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E52" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E53" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B54" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E54" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D55" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E55" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E55" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E56" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E56" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B57" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E57" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E57" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>6</v>
@@ -1465,9 +1465,77 @@
         <v>11</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="E58" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E59" s="10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E62" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1490,13 +1558,13 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="D7:D8 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.0242914979757"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>

</xml_diff>